<commit_message>
Subida de Documentación Mockup
</commit_message>
<xml_diff>
--- a/Entrega 1 (29 Octubre)/Documentación Trabajo Colaborativo/comparativa herramientas tracking time.xlsx
+++ b/Entrega 1 (29 Octubre)/Documentación Trabajo Colaborativo/comparativa herramientas tracking time.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\VScode Workspace\gitHub\Entrega 1 (29 Octubre)\Documentación Trabajo Colaborativo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5473DD9-EE32-4BD8-B06D-ED6120F44D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBF73DB-06D1-4527-AD8B-7C7B00F76840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{36B9EAF8-4169-4F56-9777-8826820E39C1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{36B9EAF8-4169-4F56-9777-8826820E39C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="16">
   <si>
     <t>✓</t>
   </si>
@@ -61,9 +61,6 @@
     <t>WakaTime</t>
   </si>
   <si>
-    <t>Admite Release+Report+Burndown</t>
-  </si>
-  <si>
     <t>Harvest</t>
   </si>
   <si>
@@ -77,14 +74,28 @@
   </si>
   <si>
     <t>DeskTime</t>
+  </si>
+  <si>
+    <t>clockify</t>
+  </si>
+  <si>
+    <t>Admite Release+Report detailed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -112,9 +123,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -431,22 +448,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A5EB30-1078-4699-83BB-0CE22C12710D}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="24.28515625" defaultRowHeight="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="24.26953125" defaultRowHeight="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="24.28515625" style="1"/>
-    <col min="5" max="5" width="35.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" style="1"/>
-    <col min="7" max="7" width="27.42578125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="24.28515625" style="1"/>
+    <col min="1" max="4" width="24.26953125" style="1"/>
+    <col min="5" max="5" width="35.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.26953125" style="1"/>
+    <col min="7" max="7" width="27.453125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="24.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="69.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -454,22 +471,22 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -492,7 +509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -515,9 +532,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -525,8 +542,8 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -538,57 +555,77 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>2</v>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>1</v>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" display="https://desktime.com/" xr:uid="{A102CC35-EDE0-48EA-A38D-82991DBCC0EA}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>